<commit_message>
aggiornamento checklist rif. email Progetto FSE 2.0 del 08/09/2023
aggiornata la descrizione della colonna "Gestione Errore" relativamente ai seguenti id test: 29, 31, 32, 37, 39, 40, 63, 65, 75, 77, 151, 153
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONNECTINFORMATICSSRL/Connect_Informatics_SRL/Equipe_FSE_Gateway/V1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111CONNECTINFORMATICSSRL/Connect_Informatics_SRL/Equipe_FSE_Gateway/V1.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectinformaticssrl.sharepoint.com/sites/NewFeaturesImprovements/Documenti condivisi/_DocRepository/GOAL/GOAL-328 FSE Accreditamento Fase 1/PULL_Request_CONNECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="812" documentId="8_{B4CEC7C5-5AC0-497F-9276-EBB40AD77860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{279DCFCF-C419-48C7-9612-3B31A2AA96F3}"/>
+  <xr:revisionPtr revIDLastSave="899" documentId="8_{B4CEC7C5-5AC0-497F-9276-EBB40AD77860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3BC92E1-AB48-400C-89A1-63DDC4E7AA94}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="483">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1490,9 +1490,6 @@
     <t>2023-08-11T08:15:17Z</t>
   </si>
   <si>
-    <t>Tramite apposito cruscotto sul software di Equipe potrà essere preso in carico l'errore, corretto il campo da interfaccia e reinviato il referto.</t>
-  </si>
-  <si>
     <t>2023-08-11T08:41:30Z</t>
   </si>
   <si>
@@ -2000,13 +1997,91 @@
   </si>
   <si>
     <t>2023-08-18T12:48:49Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L'utente medico ha comunque la possibilità di completare il documento in termini clinici. Per quanto riguarda l'inoltro al gateway dovrà attendere specifica comunicazione da parte dell'help desk aziendale che si sarà fatto carico della gestione e risoluzione del problema utilizzando le funzionalità esposte da un apposito  cruscotto di monitoraggio implementato sul sotware Equipe. Tutti i documenti prodotti dal medico in presenza dell'errore, saranno accodati e quindi saranno successivamente inviati alla risoluzione dell'errore stesso attingendo alla coda dei documenti</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> L'utente medico ha comunque la possibilità di completare il documento in termini clinici. Per quanto riguarda l'inoltro al gateway dovrà attendere specifica comunicazione da parte dell'help desk aziendale che si sarà fatto carico della gestione e risoluzione del problema utilizzando le funzionalità esposte da un apposito  cruscotto di monitoraggio implementato sul sotware Equipe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Tutti i documenti prodotti dal medico in presenza dell'errore, saranno accodati e quindi saranno successivamente inviati alla risoluzione dell'errore stesso attingendo alla coda dei documenti</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  L'utente medico ha comunque la possibilità di completare il documento in termini clinici. Per quanto riguarda l'inoltro al gateway dovrà attendere specifica comunicazione da parte dell'help desk aziendale che si sarà fatto carico della gestione e risoluzione del problema utilizzando le funzionalità esposte da un apposito  cruscotto di monitoraggio implementato sul sotware Equipe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Tutti i documenti prodotti dal medico in presenza dell'errore, saranno accodati e quindi saranno successivamente inviati alla risoluzione dell'errore stesso attingendo alla coda dei documenti</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   L'utente medico ha comunque la possibilità di completare il documento in termini clinici. Per quanto riguarda l'inoltro al gateway dovrà attendere specifica comunicazione da parte dell'help desk aziendale che si sarà fatto carico della gestione e risoluzione del problema utilizzando le funzionalità esposte da un apposito  cruscotto di monitoraggio implementato sul sotware Equipe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Tutti i documenti prodotti dal medico in presenza dell'errore, saranno accodati e quindi saranno successivamente inviati alla risoluzione dell'errore stesso attingendo alla coda dei documenti</t>
+    </r>
+  </si>
+  <si>
+    <t>La comparsa di questo errore è molto rara in quanto a livello applicativo l'obbligatorietà della clausola di riservatezza è un dato necessario. Contemplando però la presenza di ipotetici bug, tramite apposito cruscotto sul software Equipe l'help desk riconoscerà le cause del bug e, una volta corretto, permetterà al medico di riformalizzare il documento affiché sia possibile reinviarlo e quindi effettuare la validazione.</t>
+  </si>
+  <si>
+    <t>La comparsa di questo errore è molto rara in quanto a livello applicativo l'obbligatorietà e correttezza formale della clausola di riservatezza è un dato necessario. Contemplando però la presenza di ipotetici bug, tramite apposito cruscotto sul software Equipe l'help desk riconoscerà le cause del bug e, una volta corretto, permetterà al medico di riformalizzare il documento affiché sia possibile reinviarlo e quindi effettuare la validazione.</t>
+  </si>
+  <si>
+    <t>La comparsa di questo errore è molto rara in quanto a livello applicativo l'obbligatorietà  e correttezza formale della clausola di riservatezza è un dato necessario. Contemplando però la presenza di ipotetici bug, tramite apposito cruscotto sul software Equipe l'help desk riconoscerà le cause del bug e, una volta corretto, permetterà al medico di riformalizzare il documento affiché sia possibile reinviarlo e quindi effettuare la validazione.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2081,6 +2156,11 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2345,7 +2425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2477,6 +2557,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4937,10 +5020,10 @@
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="J17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -5216,13 +5299,13 @@
         <v>45155</v>
       </c>
       <c r="G10" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="I10" s="24" t="s">
         <v>411</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>412</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>84</v>
@@ -5264,7 +5347,7 @@
         <v>242</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
@@ -5302,7 +5385,7 @@
         <v>242</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
@@ -5340,7 +5423,7 @@
         <v>242</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -5374,13 +5457,13 @@
         <v>45155</v>
       </c>
       <c r="G14" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="H14" s="24" t="s">
         <v>343</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="I14" s="24" t="s">
         <v>344</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>345</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>84</v>
@@ -5418,13 +5501,13 @@
         <v>45155</v>
       </c>
       <c r="G15" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="H15" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="I15" s="24" t="s">
         <v>347</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>348</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>84</v>
@@ -5466,7 +5549,7 @@
         <v>242</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -5504,7 +5587,7 @@
         <v>242</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -5518,7 +5601,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="18" spans="1:20" ht="245.4" thickBot="1">
       <c r="A18" s="20">
         <v>29</v>
       </c>
@@ -5538,10 +5621,10 @@
         <v>45155</v>
       </c>
       <c r="G18" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>414</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>415</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>245</v>
@@ -5557,13 +5640,13 @@
         <v>84</v>
       </c>
       <c r="N18" s="25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="O18" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P18" s="25" t="s">
-        <v>417</v>
+      <c r="P18" s="52" t="s">
+        <v>476</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -5572,7 +5655,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="19" spans="1:20" ht="245.4" thickBot="1">
       <c r="A19" s="20">
         <v>31</v>
       </c>
@@ -5592,10 +5675,10 @@
         <v>45155</v>
       </c>
       <c r="G19" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="H19" s="24" t="s">
         <v>351</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>352</v>
       </c>
       <c r="I19" s="24" t="s">
         <v>245</v>
@@ -5611,13 +5694,13 @@
         <v>84</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P19" s="25" t="s">
-        <v>257</v>
+      <c r="P19" s="52" t="s">
+        <v>476</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -5626,7 +5709,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="20" spans="1:20" ht="245.4" thickBot="1">
       <c r="A20" s="20">
         <v>32</v>
       </c>
@@ -5670,8 +5753,8 @@
       <c r="O20" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P20" s="33" t="s">
-        <v>257</v>
+      <c r="P20" s="52" t="s">
+        <v>476</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -5680,7 +5763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="144.6" thickBot="1">
+    <row r="21" spans="1:20" ht="245.4" thickBot="1">
       <c r="A21" s="20">
         <v>37</v>
       </c>
@@ -5700,10 +5783,10 @@
         <v>45155</v>
       </c>
       <c r="G21" s="24" t="s">
+        <v>417</v>
+      </c>
+      <c r="H21" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>419</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>245</v>
@@ -5719,13 +5802,13 @@
         <v>84</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P21" s="25" t="s">
-        <v>417</v>
+      <c r="P21" s="33" t="s">
+        <v>477</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -5734,7 +5817,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="144.6" thickBot="1">
+    <row r="22" spans="1:20" ht="245.4" thickBot="1">
       <c r="A22" s="20">
         <v>39</v>
       </c>
@@ -5754,10 +5837,10 @@
         <v>45155</v>
       </c>
       <c r="G22" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="H22" s="24" t="s">
         <v>354</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>355</v>
       </c>
       <c r="I22" s="24" t="s">
         <v>245</v>
@@ -5773,13 +5856,13 @@
         <v>84</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O22" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P22" s="25" t="s">
-        <v>257</v>
+      <c r="P22" s="33" t="s">
+        <v>478</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
@@ -5788,7 +5871,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="144.6" thickBot="1">
+    <row r="23" spans="1:20" ht="245.4" thickBot="1">
       <c r="A23" s="20">
         <v>40</v>
       </c>
@@ -5833,7 +5916,7 @@
         <v>84</v>
       </c>
       <c r="P23" s="33" t="s">
-        <v>257</v>
+        <v>479</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="26"/>
@@ -5862,7 +5945,7 @@
         <v>45155</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
@@ -5877,13 +5960,13 @@
         <v>84</v>
       </c>
       <c r="N24" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="O24" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="P24" s="25" t="s">
         <v>422</v>
-      </c>
-      <c r="O24" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="P24" s="25" t="s">
-        <v>423</v>
       </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="26"/>
@@ -5912,7 +5995,7 @@
         <v>45155</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
@@ -5927,13 +6010,13 @@
         <v>84</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="O25" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="26"/>
@@ -5977,13 +6060,13 @@
         <v>84</v>
       </c>
       <c r="N26" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="O26" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="P26" s="25" t="s">
         <v>358</v>
-      </c>
-      <c r="O26" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="P26" s="25" t="s">
-        <v>359</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
@@ -5992,7 +6075,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="115.8" thickBot="1">
+    <row r="27" spans="1:20" ht="173.4" thickBot="1">
       <c r="A27" s="20">
         <v>63</v>
       </c>
@@ -6005,20 +6088,20 @@
       <c r="D27" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="36" t="s">
         <v>89</v>
       </c>
       <c r="F27" s="23">
         <v>45155</v>
       </c>
       <c r="G27" s="24" t="s">
+        <v>423</v>
+      </c>
+      <c r="H27" s="24" t="s">
         <v>424</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="I27" s="24" t="s">
         <v>425</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>426</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>84</v>
@@ -6031,13 +6114,13 @@
         <v>84</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>427</v>
-      </c>
-      <c r="P27" s="25" t="s">
-        <v>417</v>
+        <v>426</v>
+      </c>
+      <c r="P27" s="52" t="s">
+        <v>480</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -6066,13 +6149,13 @@
         <v>45155</v>
       </c>
       <c r="G28" s="24" t="s">
+        <v>427</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>428</v>
       </c>
-      <c r="H28" s="24" t="s">
+      <c r="I28" s="24" t="s">
         <v>429</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>430</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>84</v>
@@ -6085,13 +6168,13 @@
         <v>84</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O28" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="26"/>
@@ -6100,7 +6183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="115.8" thickBot="1">
+    <row r="29" spans="1:20" ht="187.8" thickBot="1">
       <c r="A29" s="20">
         <v>65</v>
       </c>
@@ -6120,13 +6203,13 @@
         <v>45155</v>
       </c>
       <c r="G29" s="24" t="s">
+        <v>431</v>
+      </c>
+      <c r="H29" s="24" t="s">
         <v>432</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="I29" s="24" t="s">
         <v>433</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>434</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>84</v>
@@ -6139,13 +6222,13 @@
         <v>84</v>
       </c>
       <c r="N29" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O29" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P29" s="25" t="s">
-        <v>417</v>
+      <c r="P29" s="52" t="s">
+        <v>481</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="26"/>
@@ -6174,13 +6257,13 @@
         <v>45155</v>
       </c>
       <c r="G30" s="24" t="s">
+        <v>435</v>
+      </c>
+      <c r="H30" s="24" t="s">
         <v>436</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="I30" s="24" t="s">
         <v>437</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>438</v>
       </c>
       <c r="J30" s="25" t="s">
         <v>84</v>
@@ -6193,13 +6276,13 @@
         <v>84</v>
       </c>
       <c r="N30" s="25" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="O30" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="26"/>
@@ -6228,13 +6311,13 @@
         <v>45155</v>
       </c>
       <c r="G31" s="24" t="s">
+        <v>439</v>
+      </c>
+      <c r="H31" s="24" t="s">
         <v>440</v>
       </c>
-      <c r="H31" s="24" t="s">
+      <c r="I31" s="24" t="s">
         <v>441</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>442</v>
       </c>
       <c r="J31" s="25" t="s">
         <v>84</v>
@@ -6247,13 +6330,13 @@
         <v>84</v>
       </c>
       <c r="N31" s="25" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="O31" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P31" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="26"/>
@@ -6282,13 +6365,13 @@
         <v>45155</v>
       </c>
       <c r="G32" s="24" t="s">
+        <v>443</v>
+      </c>
+      <c r="H32" s="24" t="s">
         <v>444</v>
       </c>
-      <c r="H32" s="24" t="s">
+      <c r="I32" s="24" t="s">
         <v>445</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>446</v>
       </c>
       <c r="J32" s="25" t="s">
         <v>84</v>
@@ -6301,13 +6384,13 @@
         <v>84</v>
       </c>
       <c r="N32" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O32" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P32" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="26"/>
@@ -6336,13 +6419,13 @@
         <v>45155</v>
       </c>
       <c r="G33" s="24" t="s">
+        <v>447</v>
+      </c>
+      <c r="H33" s="24" t="s">
         <v>448</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="I33" s="24" t="s">
         <v>449</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>450</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>84</v>
@@ -6355,13 +6438,13 @@
         <v>84</v>
       </c>
       <c r="N33" s="25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="O33" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P33" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="26"/>
@@ -6390,13 +6473,13 @@
         <v>45155</v>
       </c>
       <c r="G34" s="24" t="s">
+        <v>450</v>
+      </c>
+      <c r="H34" s="24" t="s">
         <v>451</v>
       </c>
-      <c r="H34" s="24" t="s">
+      <c r="I34" s="24" t="s">
         <v>452</v>
-      </c>
-      <c r="I34" s="24" t="s">
-        <v>453</v>
       </c>
       <c r="J34" s="25" t="s">
         <v>84</v>
@@ -6409,13 +6492,13 @@
         <v>84</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="O34" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P34" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -6448,7 +6531,7 @@
         <v>242</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
@@ -6486,7 +6569,7 @@
         <v>242</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -6520,13 +6603,13 @@
         <v>45155</v>
       </c>
       <c r="G37" s="24" t="s">
+        <v>454</v>
+      </c>
+      <c r="H37" s="24" t="s">
         <v>455</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="I37" s="24" t="s">
         <v>456</v>
-      </c>
-      <c r="I37" s="24" t="s">
-        <v>457</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>84</v>
@@ -6539,13 +6622,13 @@
         <v>84</v>
       </c>
       <c r="N37" s="25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="O37" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -6578,7 +6661,7 @@
         <v>242</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
@@ -6592,7 +6675,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="39" spans="1:20" ht="173.4" thickBot="1">
       <c r="A39" s="20">
         <v>75</v>
       </c>
@@ -6612,13 +6695,13 @@
         <v>45155</v>
       </c>
       <c r="G39" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="H39" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="H39" s="24" t="s">
+      <c r="I39" s="24" t="s">
         <v>362</v>
-      </c>
-      <c r="I39" s="24" t="s">
-        <v>363</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>84</v>
@@ -6631,13 +6714,13 @@
         <v>84</v>
       </c>
       <c r="N39" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O39" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P39" s="25" t="s">
-        <v>257</v>
+      <c r="P39" s="33" t="s">
+        <v>480</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -6666,13 +6749,13 @@
         <v>45155</v>
       </c>
       <c r="G40" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="H40" s="24" t="s">
         <v>365</v>
       </c>
-      <c r="H40" s="24" t="s">
+      <c r="I40" s="24" t="s">
         <v>366</v>
-      </c>
-      <c r="I40" s="24" t="s">
-        <v>367</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>84</v>
@@ -6685,7 +6768,7 @@
         <v>84</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O40" s="25" t="s">
         <v>84</v>
@@ -6700,7 +6783,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="101.4" thickBot="1">
+    <row r="41" spans="1:20" ht="187.8" thickBot="1">
       <c r="A41" s="20">
         <v>77</v>
       </c>
@@ -6720,13 +6803,13 @@
         <v>45155</v>
       </c>
       <c r="G41" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H41" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="H41" s="24" t="s">
+      <c r="I41" s="24" t="s">
         <v>370</v>
-      </c>
-      <c r="I41" s="24" t="s">
-        <v>371</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>84</v>
@@ -6739,13 +6822,13 @@
         <v>84</v>
       </c>
       <c r="N41" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O41" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="P41" s="25" t="s">
-        <v>257</v>
+      <c r="P41" s="33" t="s">
+        <v>482</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="26"/>
@@ -6774,13 +6857,13 @@
         <v>45155</v>
       </c>
       <c r="G42" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="H42" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="H42" s="24" t="s">
+      <c r="I42" s="24" t="s">
         <v>375</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>376</v>
       </c>
       <c r="J42" s="25" t="s">
         <v>84</v>
@@ -6793,7 +6876,7 @@
         <v>84</v>
       </c>
       <c r="N42" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="O42" s="25" t="s">
         <v>84</v>
@@ -6828,13 +6911,13 @@
         <v>45155</v>
       </c>
       <c r="G43" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="H43" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="H43" s="24" t="s">
+      <c r="I43" s="24" t="s">
         <v>379</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>380</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>84</v>
@@ -6847,7 +6930,7 @@
         <v>84</v>
       </c>
       <c r="N43" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="O43" s="25" t="s">
         <v>84</v>
@@ -6882,13 +6965,13 @@
         <v>45155</v>
       </c>
       <c r="G44" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="H44" s="24" t="s">
         <v>382</v>
       </c>
-      <c r="H44" s="24" t="s">
+      <c r="I44" s="24" t="s">
         <v>383</v>
-      </c>
-      <c r="I44" s="24" t="s">
-        <v>384</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>84</v>
@@ -6901,7 +6984,7 @@
         <v>84</v>
       </c>
       <c r="N44" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O44" s="25" t="s">
         <v>84</v>
@@ -6936,13 +7019,13 @@
         <v>45155</v>
       </c>
       <c r="G45" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="H45" s="24" t="s">
         <v>386</v>
       </c>
-      <c r="H45" s="24" t="s">
+      <c r="I45" s="24" t="s">
         <v>387</v>
-      </c>
-      <c r="I45" s="24" t="s">
-        <v>388</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>84</v>
@@ -6955,7 +7038,7 @@
         <v>84</v>
       </c>
       <c r="N45" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>84</v>
@@ -6990,13 +7073,13 @@
         <v>45155</v>
       </c>
       <c r="G46" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="H46" s="24" t="s">
         <v>390</v>
       </c>
-      <c r="H46" s="24" t="s">
+      <c r="I46" s="24" t="s">
         <v>391</v>
-      </c>
-      <c r="I46" s="24" t="s">
-        <v>392</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>84</v>
@@ -7009,7 +7092,7 @@
         <v>84</v>
       </c>
       <c r="N46" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>84</v>
@@ -7044,13 +7127,13 @@
         <v>45155</v>
       </c>
       <c r="G47" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="H47" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="I47" s="24" t="s">
         <v>395</v>
-      </c>
-      <c r="I47" s="24" t="s">
-        <v>396</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>84</v>
@@ -7063,7 +7146,7 @@
         <v>84</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>84</v>
@@ -7098,13 +7181,13 @@
         <v>45155</v>
       </c>
       <c r="G48" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="H48" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="H48" s="24" t="s">
+      <c r="I48" s="24" t="s">
         <v>399</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>400</v>
       </c>
       <c r="J48" s="25" t="s">
         <v>84</v>
@@ -7117,7 +7200,7 @@
         <v>84</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>84</v>
@@ -7152,13 +7235,13 @@
         <v>45155</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H49" s="24" t="s">
+        <v>401</v>
+      </c>
+      <c r="I49" s="24" t="s">
         <v>402</v>
-      </c>
-      <c r="I49" s="24" t="s">
-        <v>403</v>
       </c>
       <c r="J49" s="25" t="s">
         <v>84</v>
@@ -7171,7 +7254,7 @@
         <v>84</v>
       </c>
       <c r="N49" s="25" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O49" s="25" t="s">
         <v>84</v>
@@ -7210,7 +7293,7 @@
         <v>242</v>
       </c>
       <c r="K50" s="25" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L50" s="25"/>
       <c r="M50" s="25"/>
@@ -7248,7 +7331,7 @@
         <v>242</v>
       </c>
       <c r="K51" s="25" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L51" s="25"/>
       <c r="M51" s="25"/>
@@ -7286,7 +7369,7 @@
         <v>242</v>
       </c>
       <c r="K52" s="25" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L52" s="25"/>
       <c r="M52" s="25"/>
@@ -7324,7 +7407,7 @@
         <v>242</v>
       </c>
       <c r="K53" s="25" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L53" s="25"/>
       <c r="M53" s="25"/>
@@ -7362,7 +7445,7 @@
         <v>242</v>
       </c>
       <c r="K54" s="25" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L54" s="25"/>
       <c r="M54" s="25"/>
@@ -7400,7 +7483,7 @@
         <v>242</v>
       </c>
       <c r="K55" s="25" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -7438,7 +7521,7 @@
         <v>242</v>
       </c>
       <c r="K56" s="25" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L56" s="25"/>
       <c r="M56" s="25"/>
@@ -7476,7 +7559,7 @@
         <v>242</v>
       </c>
       <c r="K57" s="25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="L57" s="25"/>
       <c r="M57" s="25"/>
@@ -7648,7 +7731,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="101.4" thickBot="1">
+    <row r="62" spans="1:20" ht="173.4" thickBot="1">
       <c r="A62" s="20">
         <v>151</v>
       </c>
@@ -7693,7 +7776,7 @@
         <v>84</v>
       </c>
       <c r="P62" s="33" t="s">
-        <v>322</v>
+        <v>480</v>
       </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="26"/>
@@ -7722,7 +7805,7 @@
         <v>45149</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H63" s="34" t="s">
         <v>262</v>
@@ -7747,7 +7830,7 @@
         <v>84</v>
       </c>
       <c r="P63" s="33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="26"/>
@@ -7756,7 +7839,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="115.8" thickBot="1">
+    <row r="64" spans="1:20" ht="187.8" thickBot="1">
       <c r="A64" s="20">
         <v>153</v>
       </c>
@@ -7776,7 +7859,7 @@
         <v>45149</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H64" s="34" t="s">
         <v>265</v>
@@ -7801,7 +7884,7 @@
         <v>84</v>
       </c>
       <c r="P64" s="33" t="s">
-        <v>257</v>
+        <v>482</v>
       </c>
       <c r="Q64" s="25"/>
       <c r="R64" s="26"/>
@@ -7830,7 +7913,7 @@
         <v>45149</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H65" s="34" t="s">
         <v>268</v>
@@ -7855,7 +7938,7 @@
         <v>84</v>
       </c>
       <c r="P65" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q65" s="25"/>
       <c r="R65" s="26"/>
@@ -7884,7 +7967,7 @@
         <v>45149</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H66" s="34" t="s">
         <v>271</v>
@@ -7909,7 +7992,7 @@
         <v>84</v>
       </c>
       <c r="P66" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q66" s="25"/>
       <c r="R66" s="26"/>
@@ -7938,7 +8021,7 @@
         <v>45149</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H67" s="24" t="s">
         <v>274</v>
@@ -7963,7 +8046,7 @@
         <v>84</v>
       </c>
       <c r="P67" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="26"/>
@@ -7992,7 +8075,7 @@
         <v>45149</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H68" s="24" t="s">
         <v>277</v>
@@ -8017,7 +8100,7 @@
         <v>84</v>
       </c>
       <c r="P68" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q68" s="25"/>
       <c r="R68" s="26"/>
@@ -8046,7 +8129,7 @@
         <v>45149</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H69" s="34" t="s">
         <v>281</v>
@@ -8071,7 +8154,7 @@
         <v>84</v>
       </c>
       <c r="P69" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q69" s="25"/>
       <c r="R69" s="26"/>
@@ -8100,7 +8183,7 @@
         <v>45149</v>
       </c>
       <c r="G70" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H70" s="34" t="s">
         <v>284</v>
@@ -8125,7 +8208,7 @@
         <v>84</v>
       </c>
       <c r="P70" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q70" s="25"/>
       <c r="R70" s="26"/>
@@ -8154,7 +8237,7 @@
         <v>45149</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H71" s="34" t="s">
         <v>287</v>
@@ -8179,7 +8262,7 @@
         <v>84</v>
       </c>
       <c r="P71" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q71" s="25"/>
       <c r="R71" s="26"/>
@@ -8208,7 +8291,7 @@
         <v>45149</v>
       </c>
       <c r="G72" s="34" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H72" s="34" t="s">
         <v>290</v>
@@ -8233,7 +8316,7 @@
         <v>84</v>
       </c>
       <c r="P72" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q72" s="25"/>
       <c r="R72" s="26"/>
@@ -8262,7 +8345,7 @@
         <v>45149</v>
       </c>
       <c r="G73" s="34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H73" s="34" t="s">
         <v>293</v>
@@ -8287,7 +8370,7 @@
         <v>84</v>
       </c>
       <c r="P73" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q73" s="25"/>
       <c r="R73" s="26"/>
@@ -8316,7 +8399,7 @@
         <v>45149</v>
       </c>
       <c r="G74" s="34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H74" s="34" t="s">
         <v>296</v>
@@ -8341,7 +8424,7 @@
         <v>84</v>
       </c>
       <c r="P74" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q74" s="25"/>
       <c r="R74" s="26"/>
@@ -8370,7 +8453,7 @@
         <v>45149</v>
       </c>
       <c r="G75" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H75" s="34" t="s">
         <v>299</v>
@@ -8395,7 +8478,7 @@
         <v>84</v>
       </c>
       <c r="P75" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q75" s="25"/>
       <c r="R75" s="26"/>
@@ -8424,7 +8507,7 @@
         <v>45149</v>
       </c>
       <c r="G76" s="34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H76" s="34" t="s">
         <v>303</v>
@@ -8449,7 +8532,7 @@
         <v>84</v>
       </c>
       <c r="P76" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q76" s="25"/>
       <c r="R76" s="26"/>
@@ -8478,7 +8561,7 @@
         <v>45149</v>
       </c>
       <c r="G77" s="34" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H77" s="34" t="s">
         <v>306</v>
@@ -8503,7 +8586,7 @@
         <v>84</v>
       </c>
       <c r="P77" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q77" s="25"/>
       <c r="R77" s="26"/>
@@ -8532,7 +8615,7 @@
         <v>45149</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H78" s="24" t="s">
         <v>309</v>
@@ -8557,7 +8640,7 @@
         <v>84</v>
       </c>
       <c r="P78" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q78" s="25"/>
       <c r="R78" s="26"/>
@@ -8586,7 +8669,7 @@
         <v>45149</v>
       </c>
       <c r="G79" s="34" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H79" s="34" t="s">
         <v>312</v>
@@ -8611,7 +8694,7 @@
         <v>84</v>
       </c>
       <c r="P79" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q79" s="25"/>
       <c r="R79" s="26"/>
@@ -8640,7 +8723,7 @@
         <v>45149</v>
       </c>
       <c r="G80" s="34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H80" s="34" t="s">
         <v>314</v>
@@ -8665,7 +8748,7 @@
         <v>84</v>
       </c>
       <c r="P80" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q80" s="25"/>
       <c r="R80" s="26"/>
@@ -8685,22 +8768,22 @@
         <v>47</v>
       </c>
       <c r="D81" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="E81" s="22" t="s">
         <v>460</v>
-      </c>
-      <c r="E81" s="22" t="s">
-        <v>461</v>
       </c>
       <c r="F81" s="23">
         <v>45155</v>
       </c>
       <c r="G81" s="24" t="s">
+        <v>461</v>
+      </c>
+      <c r="H81" s="24" t="s">
         <v>462</v>
       </c>
-      <c r="H81" s="24" t="s">
+      <c r="I81" s="24" t="s">
         <v>463</v>
-      </c>
-      <c r="I81" s="24" t="s">
-        <v>464</v>
       </c>
       <c r="J81" s="25" t="s">
         <v>84</v>
@@ -8729,22 +8812,22 @@
         <v>48</v>
       </c>
       <c r="D82" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="E82" s="22" t="s">
         <v>467</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>468</v>
       </c>
       <c r="F82" s="23">
         <v>45155</v>
       </c>
       <c r="G82" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="H82" s="24" t="s">
         <v>469</v>
       </c>
-      <c r="H82" s="24" t="s">
+      <c r="I82" s="24" t="s">
         <v>470</v>
-      </c>
-      <c r="I82" s="24" t="s">
-        <v>471</v>
       </c>
       <c r="J82" s="25" t="s">
         <v>84</v>
@@ -8773,22 +8856,22 @@
         <v>52</v>
       </c>
       <c r="D83" s="21" t="s">
+        <v>471</v>
+      </c>
+      <c r="E83" s="22" t="s">
         <v>472</v>
-      </c>
-      <c r="E83" s="22" t="s">
-        <v>473</v>
       </c>
       <c r="F83" s="23">
         <v>45156</v>
       </c>
       <c r="G83" s="34" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H83" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="I83" s="34" t="s">
         <v>474</v>
-      </c>
-      <c r="I83" s="34" t="s">
-        <v>475</v>
       </c>
       <c r="J83" s="33" t="s">
         <v>84</v>
@@ -8901,7 +8984,7 @@
         <v>195</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>198</v>
@@ -8915,7 +8998,7 @@
         <v>195</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>199</v>
@@ -8971,7 +9054,7 @@
         <v>195</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>206</v>
@@ -11566,26 +11649,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4d888290-14b9-431c-8798-9717b884c822">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ec19d4eb-5c83-4fae-999e-f022a82898a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B6AF07B2DF4D634894694C40D95CAEB9" ma:contentTypeVersion="17" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="603cfe832bf4a91790e47f02d702d612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d888290-14b9-431c-8798-9717b884c822" xmlns:ns3="ec19d4eb-5c83-4fae-999e-f022a82898a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b49a15abf44b7219298daa7ba1c4cb7d" ns2:_="" ns3:_="">
     <xsd:import namespace="4d888290-14b9-431c-8798-9717b884c822"/>
@@ -11834,26 +11897,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D67A06AB-ECCA-49D8-AD4E-39A9EA2DB8D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4d888290-14b9-431c-8798-9717b884c822"/>
-    <ds:schemaRef ds:uri="ec19d4eb-5c83-4fae-999e-f022a82898a7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F9FDCFA-6988-4E51-BFC7-3EC8B09150D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4d888290-14b9-431c-8798-9717b884c822">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ec19d4eb-5c83-4fae-999e-f022a82898a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AC46678-D4D6-4AF4-A135-46AEAAF7F56A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11870,4 +11934,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F9FDCFA-6988-4E51-BFC7-3EC8B09150D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D67A06AB-ECCA-49D8-AD4E-39A9EA2DB8D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4d888290-14b9-431c-8798-9717b884c822"/>
+    <ds:schemaRef ds:uri="ec19d4eb-5c83-4fae-999e-f022a82898a7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>